<commit_message>
Stage 1-2 : Task A1-A20 Evidence
</commit_message>
<xml_diff>
--- a/arnettee/evidence.xlsx
+++ b/arnettee/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Drive'ım\Coin\Testnet\game-of-nfts\arnettee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kivo\Drive'ım\Coin\Testnet\game-of-nfts\arnettee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD743763-5973-432E-8D63-3F926C0644B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B2A66-6A19-426B-B520-79105724A831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -164,13 +149,166 @@
   </si>
   <si>
     <t>DC9E80686570D314A565812FB57E4730D900305FA589879D9C5A03523BF467A6</t>
+  </si>
+  <si>
+    <t>ibc/0F6FEF42870BD3C0C3D567F1243992EE485DB9E77CD923012C8674FFED8FC6BD</t>
+  </si>
+  <si>
+    <t>nftid08</t>
+  </si>
+  <si>
+    <t>ibc/BD5A2D7149F0F6EED56BC891F34ACF98ACA020A14B0E177D886299061DE9B7E5</t>
+  </si>
+  <si>
+    <t>ibc/21965A8C29D255E9DE0D9D65BE4D5602F61933B30F9B7158E9E544C7FECBB3F1</t>
+  </si>
+  <si>
+    <t>nftid10</t>
+  </si>
+  <si>
+    <t>nftid09</t>
+  </si>
+  <si>
+    <t>ibc/FE0D81AAEF7646637536D09C7850A1AE6BDCE7408899EBBC0B0060067E996143</t>
+  </si>
+  <si>
+    <t>nftid11</t>
+  </si>
+  <si>
+    <t>ibc/19EE17C815D764780E48C05D2311471FCC883558ADEC97FDA3411E45187A4372</t>
+  </si>
+  <si>
+    <t>nftid12</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>8912CF5B3CFD43A3C9910DF7AB34986B8FBD7EAED038B3B2DBA4F6E8AD6FF3B1</t>
+  </si>
+  <si>
+    <t>378DFF769313459F99AED24B93324E9086EFA6F54F5E9951226D2DF680578766</t>
+  </si>
+  <si>
+    <t>68D727454017519668C1806220FCE343C1CA4F1AA46322840D7416AE588B8548</t>
+  </si>
+  <si>
+    <t>29EAD33CA756C61849B15AE43CF61CB93502941FB9985058AAD59843756D571F</t>
+  </si>
+  <si>
+    <t>5F16CF0F8C4B1EC23AFD5BEB2382BC21760D5D300CAF258EA263FBF3B90D256F</t>
+  </si>
+  <si>
+    <t>0418BA204C445234329CA6865567D3A3A3B811C8E5C693D289DE33F60C8FF67E</t>
+  </si>
+  <si>
+    <t>84931E95E977C3118823CE6139113832ADC9709D375A8D32F1B84E8E5F8C689C</t>
+  </si>
+  <si>
+    <t>DD2CA241B939C40A1D19BB9EAB7666BA17AD60E6E1AD26C8CA4DE0DC37E56439</t>
+  </si>
+  <si>
+    <t>47776EFE01E7360D1F5324FFBBCCB60EF35FE70E274A19C1495C7771FBB804FD</t>
+  </si>
+  <si>
+    <t>2D6B0E49C9ADCF2E11EEB628C316A34BEA373DB6461E5CBF7B654CB1D6B5FD35</t>
+  </si>
+  <si>
+    <t>C3414BE75DF88C987B8A329DFE31DFC7670CBCDCF2BE1F0F36D19A065BD4B4A4</t>
+  </si>
+  <si>
+    <t>7E5F4D9F268718D965381BE454FEE72BFF512745C5FC31DF15A0B9E40E6B873E</t>
+  </si>
+  <si>
+    <t>C4A4051A916A51C266142BE55B96BD06872BEEAEF840CC8791D54277C75D5425</t>
+  </si>
+  <si>
+    <t>BBA4523E517097E6B7EA3E189DD641B63D861E3FFB570BA52C0917DCBC5E3A89</t>
+  </si>
+  <si>
+    <t>CD4550FC3A4890D09F11685FBC5C863358D619BCF042E5E8FCDE262367D39DE4</t>
+  </si>
+  <si>
+    <t>98AC08B381F49E4D038A31EB587176DB8F821027252C9259CDBE282EAE7BF866</t>
+  </si>
+  <si>
+    <t>3D03A1E9EE956F032731F4FF0C461FF93DEB6988CB0B6D5D4D7F39F78E0FF8C6</t>
+  </si>
+  <si>
+    <t>5F48F0D0B2D030536921B93311405385A730D54747BEA8D6BDE4E22BC1F6B9B0</t>
+  </si>
+  <si>
+    <t>F645070613B1F4C29973B849E5F67722F67EDEFAE23CE08E9A651119F95D1BF4</t>
+  </si>
+  <si>
+    <t>E85A25530E1627F6FA648C402C5D1F961A6F75628FA32AA2FDC8AF25995C943B</t>
+  </si>
+  <si>
+    <t>4E947AC615CF71B96079384FF17F28A26FCEF1CF44227F9041A360ED1F0B7EFE</t>
+  </si>
+  <si>
+    <t>32B2C746222C42AB78CB33A907368D81CB5C6AA0E787186790AF7CBA028879ED</t>
+  </si>
+  <si>
+    <t>DADCC257FA3E17761641B4554EDFC32761D1CF51D9C81CB181B6F2CA09C9043E</t>
+  </si>
+  <si>
+    <t>885B70D3C06FE69D864323F57D32DE05A1856E6742EF15C4B6F9B4B3449C64B1</t>
+  </si>
+  <si>
+    <t>BB318D85E906392CEC18E194783CBA45A492DAECC7779ED473054A09432005D3</t>
+  </si>
+  <si>
+    <t>F190970E4A76975EFF5D73AFD1A636282047CCB5EF6B945452669C72F0F2E9E4</t>
+  </si>
+  <si>
+    <t>7EA61B3DEDA4A0EF0A457EC35F6C895C99538478C23EFEB9DADB0DA3CCE1B8F2</t>
+  </si>
+  <si>
+    <t>3A602F47FB0110F047FDE3CB91ECB676DAAA90B772979260826D17BADBDD7522</t>
+  </si>
+  <si>
+    <t>23E60F9295445706DF51B4EF6E428EA8E1AB710ED636DA8DFF2253C24C76FB21</t>
+  </si>
+  <si>
+    <t>25AEBAB2BF24229042204C10D33AF5A3445270265020D844F9E96CD8E9D7241E</t>
+  </si>
+  <si>
+    <t>5A287655A542A398943B849C305965362553180ACE8DD66492B4F156A5CBF91C</t>
+  </si>
+  <si>
+    <t>DE07A477BCC7F813F295F66070FBCFA1398FEB0D19AB527B36A88AADA3898E88</t>
+  </si>
+  <si>
+    <t>6CD6D7B037BECC45758FF6855C7F5419B427CC5C06A5AAEAE7F4988633919C15</t>
+  </si>
+  <si>
+    <t>B07C2FFB4A19DE648D35BE8645C3BC4C7AA88AD375E2F0EB22AD812A0296CF03</t>
+  </si>
+  <si>
+    <t>0E848ADB539FE8EF6B0D6EC91E0222AC5826942FBD2A2176441240B4E64FC725</t>
+  </si>
+  <si>
+    <t>824ADA205A0933E53FCC845C7A07214E79865FBCAF314A4FB4FA8B305A8A7904</t>
+  </si>
+  <si>
+    <t>nfid0007</t>
+  </si>
+  <si>
+    <t>ibc/A66B861BC6EB88B0202F78075E6698AE2CE1E58835E983BCE29511CD3AC8F168</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +328,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -241,10 +386,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -259,9 +412,56 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4582DF37-E76A-4292-ADDE-E2C74AA051F8}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{FBF15F81-C364-4C20-8268-408B3318CAE1}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{B2536CC1-731B-4ABA-AF68-C2E177C35DB8}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{15D974FC-D126-40CF-9228-DE3F254C1C88}"/>
+    <cellStyle name="Normal 6" xfId="5" xr:uid="{F418B892-0D73-44F0-8567-0B5A72018E57}"/>
+    <cellStyle name="Normal 7" xfId="6" xr:uid="{19CC13C7-F5CB-4A8D-868D-B00454601B81}"/>
+    <cellStyle name="Normal 8" xfId="7" xr:uid="{D1EE9E44-3F21-4E95-ADE5-2233AAD4925F}"/>
+    <cellStyle name="Normal 9" xfId="8" xr:uid="{4FB597DA-A622-420A-A451-97BC54D64A0B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,69 +766,69 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -643,28 +843,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="82.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -679,28 +881,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="81.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -715,28 +919,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="81.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -751,28 +957,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="80.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -785,17 +993,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,22 +1013,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -831,17 +1055,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="77.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,22 +1075,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>53</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -877,17 +1117,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="80.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,22 +1137,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>57</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -923,17 +1179,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="78.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,22 +1199,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -969,17 +1241,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="78.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -987,22 +1261,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>65</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1015,17 +1303,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="79.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,22 +1323,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1067,26 +1371,26 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="84.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="84.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1099,17 +1403,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="68.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,22 +1423,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1145,17 +1481,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,22 +1501,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1195,22 +1563,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1229,22 +1597,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1263,22 +1631,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1297,22 +1665,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1333,44 +1701,44 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="84.7109375" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="84.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1390,92 +1758,92 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="83.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="83.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1494,40 +1862,40 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="82.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="82.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1546,40 +1914,40 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="83.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1594,28 +1962,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="81.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1630,28 +2000,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="82.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>